<commit_message>
data translation layer updates - need to be prepped for transition
</commit_message>
<xml_diff>
--- a/backup_data_storage.xlsx
+++ b/backup_data_storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorross/Desktop/My Projects/bettingatwork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645200EF-C111-A847-A6DE-6D006882E170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD5F2D8-E93E-8D43-911C-DA95CB854E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="11" activeTab="25" xr2:uid="{16EFE6C4-92B7-6541-967E-29AAF9B7C019}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="15" activeTab="26" xr2:uid="{16EFE6C4-92B7-6541-967E-29AAF9B7C019}"/>
   </bookViews>
   <sheets>
     <sheet name="5.3.2021" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,8 @@
     <sheet name="10.04.2021" sheetId="30" r:id="rId24"/>
     <sheet name="10.11.2021" sheetId="31" r:id="rId25"/>
     <sheet name="10.18.2021" sheetId="32" r:id="rId26"/>
-    <sheet name="bets_9.20" sheetId="28" state="hidden" r:id="rId27"/>
+    <sheet name="10.25.2021" sheetId="33" r:id="rId27"/>
+    <sheet name="bets_9.20" sheetId="28" state="hidden" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3017" uniqueCount="275">
   <si>
     <t>Agent</t>
   </si>
@@ -867,13 +868,31 @@
   </si>
   <si>
     <t>remainder</t>
+  </si>
+  <si>
+    <t>ok so -700 from monster teaser, -50 from 7 pick parlay, -250 from 7 point teaser, +500 from 13 point monster, -700 from virginia monster, +500 from penn st alternate, -750 from colts ml, -600 on bengals teaser, -250 on colts parlay, jags teaser is still alive</t>
+  </si>
+  <si>
+    <t>we each pay christian $21 total, $21 for kickbacks and $0 for 5 active players</t>
+  </si>
+  <si>
+    <t>amount paid</t>
+  </si>
+  <si>
+    <t>amount left</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>Oustanding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -949,6 +968,13 @@
       <color rgb="FF555555"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1535,10 +1561,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1787,17 +1814,35 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="10" fillId="16" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -2211,16 +2256,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2243,7 +2288,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6096000" y="596900"/>
+          <a:off x="5829300" y="711200"/>
           <a:ext cx="6921500" cy="2590800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2261,15 +2306,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>256822</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>49388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:colOff>561622</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>121355</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2292,8 +2337,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5308600" y="596900"/>
-          <a:ext cx="6908800" cy="2578100"/>
+          <a:off x="5576711" y="656166"/>
+          <a:ext cx="6965244" cy="2513189"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2309,16 +2354,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28223</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>14111</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>536223</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>56444</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>52211</xdr:rowOff>
+      <xdr:colOff>259645</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>94544</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2341,7 +2386,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6180667" y="1467555"/>
+          <a:off x="5856112" y="1312333"/>
           <a:ext cx="3886200" cy="1816100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2392,6 +2437,55 @@
         <a:xfrm>
           <a:off x="5943600" y="876300"/>
           <a:ext cx="3898900" cy="2552700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>522111</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>111478</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>172156</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>162278</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18906F41-9CDC-394F-8C72-7A461047165B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7239000" y="1169811"/>
+          <a:ext cx="3812823" cy="1842911"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9639,7 +9733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2739710E-14F1-464B-A50D-878A173AA683}">
   <dimension ref="B2:U40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:F40"/>
     </sheetView>
   </sheetViews>
@@ -10567,8 +10661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43CA7AE-8493-2B44-A730-231869841FAA}">
   <dimension ref="B3:P42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12051,15 +12145,16 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8E9F75-CFC4-834B-91E8-E0F7C8A11E90}">
-  <dimension ref="B3:O49"/>
+  <dimension ref="B3:O78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="79" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:15" ht="17" thickBot="1"/>
@@ -12304,7 +12399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:13">
       <c r="B17" s="90" t="s">
         <v>17</v>
       </c>
@@ -12321,7 +12416,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:13">
       <c r="B18" s="90" t="s">
         <v>17</v>
       </c>
@@ -12338,7 +12433,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="17" thickBot="1">
+    <row r="19" spans="2:13" ht="17" thickBot="1">
       <c r="B19" s="93" t="s">
         <v>17</v>
       </c>
@@ -12355,7 +12450,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:13">
       <c r="B20" s="102" t="s">
         <v>27</v>
       </c>
@@ -12372,7 +12467,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:13">
       <c r="B21" s="102" t="s">
         <v>27</v>
       </c>
@@ -12388,8 +12483,11 @@
       <c r="F21" s="104">
         <v>364</v>
       </c>
-    </row>
-    <row r="22" spans="2:9">
+      <c r="M21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" s="102" t="s">
         <v>27</v>
       </c>
@@ -12406,7 +12504,7 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:13">
       <c r="B23" s="102" t="s">
         <v>27</v>
       </c>
@@ -12423,7 +12521,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:13">
       <c r="B24" s="102" t="s">
         <v>27</v>
       </c>
@@ -12440,7 +12538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:13">
       <c r="B25" s="102" t="s">
         <v>27</v>
       </c>
@@ -12457,7 +12555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:13">
       <c r="B26" s="102" t="s">
         <v>27</v>
       </c>
@@ -12474,7 +12572,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:13">
       <c r="B27" s="102" t="s">
         <v>27</v>
       </c>
@@ -12491,7 +12589,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:13">
       <c r="B28" s="102" t="s">
         <v>27</v>
       </c>
@@ -12508,7 +12606,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:13">
       <c r="B29" s="102" t="s">
         <v>27</v>
       </c>
@@ -12525,7 +12623,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:13">
       <c r="B30" s="102" t="s">
         <v>27</v>
       </c>
@@ -12542,7 +12640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:13">
       <c r="B31" s="102" t="s">
         <v>27</v>
       </c>
@@ -12559,7 +12657,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="17" thickBot="1">
+    <row r="32" spans="2:13" ht="17" thickBot="1">
       <c r="B32" s="105" t="s">
         <v>27</v>
       </c>
@@ -12582,7 +12680,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:13">
       <c r="B33" s="122" t="s">
         <v>40</v>
       </c>
@@ -12609,7 +12707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:13">
       <c r="B34" s="122" t="s">
         <v>40</v>
       </c>
@@ -12636,7 +12734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:13">
       <c r="B35" s="122" t="s">
         <v>40</v>
       </c>
@@ -12663,7 +12761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:13">
       <c r="B36" s="122" t="s">
         <v>40</v>
       </c>
@@ -12690,7 +12788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:13">
       <c r="B37" s="122" t="s">
         <v>40</v>
       </c>
@@ -12716,8 +12814,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:9">
+      <c r="M37">
+        <f>190-300</f>
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13">
       <c r="B38" s="122" t="s">
         <v>40</v>
       </c>
@@ -12743,8 +12845,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:9">
+      <c r="M38">
+        <f>-450+158</f>
+        <v>-292</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13">
       <c r="B39" s="122" t="s">
         <v>40</v>
       </c>
@@ -12771,7 +12877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:13">
       <c r="B40" s="122" t="s">
         <v>40</v>
       </c>
@@ -12798,7 +12904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:13">
       <c r="B41" s="122" t="s">
         <v>40</v>
       </c>
@@ -12825,7 +12931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:13">
       <c r="B42" s="122" t="s">
         <v>40</v>
       </c>
@@ -12852,7 +12958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:9">
+    <row r="43" spans="2:13">
       <c r="B43" s="122" t="s">
         <v>40</v>
       </c>
@@ -12879,7 +12985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:13">
       <c r="B44" s="122" t="s">
         <v>40</v>
       </c>
@@ -12906,7 +13012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:13">
       <c r="B45" s="122" t="s">
         <v>40</v>
       </c>
@@ -12933,7 +13039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="17" thickBot="1">
+    <row r="46" spans="2:13" ht="17" thickBot="1">
       <c r="B46" s="124" t="s">
         <v>40</v>
       </c>
@@ -12953,17 +13059,28 @@
         <v>261</v>
       </c>
       <c r="H46">
-        <v>500</v>
+        <v>1012.5</v>
       </c>
       <c r="I46" s="219">
         <f t="shared" si="0"/>
-        <v>512.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="12:12">
       <c r="L49">
         <f>SUM(I37:I46)</f>
-        <v>512.5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="14:14" ht="409.6">
+      <c r="N70" s="220" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="78" spans="14:14">
+      <c r="N78">
+        <f>-700-50-250+500-700+500-750-600-250</f>
+        <v>-2300</v>
       </c>
     </row>
   </sheetData>
@@ -12973,6 +13090,916 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD38A5F-3C98-D345-BA08-528606904ED0}">
+  <dimension ref="B3:P44"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:16" ht="17" thickBot="1"/>
+    <row r="4" spans="2:16" ht="20" thickBot="1">
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="221" t="s">
+        <v>264</v>
+      </c>
+      <c r="I4" s="222"/>
+      <c r="J4" s="222"/>
+      <c r="K4" s="222"/>
+      <c r="L4" s="222"/>
+      <c r="M4" s="222"/>
+      <c r="N4" s="222"/>
+      <c r="O4" s="222"/>
+      <c r="P4" s="222"/>
+    </row>
+    <row r="5" spans="2:16">
+      <c r="B5" s="127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="128" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="128" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="128" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="129">
+        <v>130</v>
+      </c>
+      <c r="H5" s="221" t="s">
+        <v>270</v>
+      </c>
+      <c r="I5" s="222"/>
+      <c r="J5" s="222"/>
+      <c r="K5" s="222"/>
+      <c r="L5" s="222"/>
+      <c r="M5" s="222"/>
+      <c r="N5" s="222"/>
+      <c r="O5" s="222"/>
+      <c r="P5" s="222"/>
+    </row>
+    <row r="6" spans="2:16">
+      <c r="B6" s="137" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="136" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="136" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="136" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="17" thickBot="1">
+      <c r="B7" s="130" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="131" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="131" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" s="131" t="s">
+        <v>229</v>
+      </c>
+      <c r="F7" s="132">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
+      <c r="B8" s="109" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="110" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="110" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="111">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
+      <c r="B9" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="B10" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="92">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
+      <c r="B11" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="91" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
+      <c r="B12" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="91" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="91" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
+      <c r="B13" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="92">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
+      <c r="B14" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="92">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
+      <c r="B15" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="92">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="B16" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="91" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="91" t="s">
+        <v>250</v>
+      </c>
+      <c r="F16" s="92">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="B17" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="91" t="s">
+        <v>251</v>
+      </c>
+      <c r="E17" s="91" t="s">
+        <v>252</v>
+      </c>
+      <c r="F17" s="92">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="17" thickBot="1">
+      <c r="B18" s="93" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="94" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="E18" s="94" t="s">
+        <v>254</v>
+      </c>
+      <c r="F18" s="95">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="100" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="101">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="103" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="103" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="104">
+        <v>0</v>
+      </c>
+      <c r="O20" s="223">
+        <f>3237/5208</f>
+        <v>0.62154377880184331</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="B21" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="103" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="103" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="104">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16">
+      <c r="B22" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="103" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="104">
+        <v>1269.9000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16">
+      <c r="B23" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="103" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="103" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="104">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16">
+      <c r="B24" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="103" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="103" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="104">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="B25" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="103" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="103" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="104">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="B26" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="103" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="103" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="104">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16">
+      <c r="B27" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="103" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="104">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="103" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="103" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="104">
+        <v>315</v>
+      </c>
+      <c r="K28" t="s">
+        <v>274</v>
+      </c>
+      <c r="P28">
+        <f>1481/5208</f>
+        <v>0.28437019969278032</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="103" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" s="104">
+        <v>25</v>
+      </c>
+      <c r="K29">
+        <f>SUM(I31:I44)</f>
+        <v>3839.1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="17" thickBot="1">
+      <c r="B30" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="106" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="106" t="s">
+        <v>244</v>
+      </c>
+      <c r="E30" s="106" t="s">
+        <v>245</v>
+      </c>
+      <c r="F30" s="107">
+        <v>1083.5999999999999</v>
+      </c>
+      <c r="G30" s="218" t="s">
+        <v>273</v>
+      </c>
+      <c r="H30" s="218" t="s">
+        <v>271</v>
+      </c>
+      <c r="I30" s="218" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16">
+      <c r="B31" s="133" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="134" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="134" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="134" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="135">
+        <v>138</v>
+      </c>
+      <c r="G31" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H31">
+        <v>138</v>
+      </c>
+      <c r="I31">
+        <f>IF(C31="Pay",H31-F31,F31-H31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16">
+      <c r="B32" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="118" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="118" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="118" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="123">
+        <v>351</v>
+      </c>
+      <c r="G32" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H32">
+        <v>351</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32:I44" si="0">IF(C32="Pay",H32-F32,F32-H32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="118" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="118" t="s">
+        <v>257</v>
+      </c>
+      <c r="E33" s="118" t="s">
+        <v>258</v>
+      </c>
+      <c r="F33" s="123">
+        <v>257</v>
+      </c>
+      <c r="G33" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H33">
+        <v>257</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="118" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="118" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="123">
+        <v>446</v>
+      </c>
+      <c r="G34" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H34">
+        <v>446</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="118" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="118" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="123">
+        <v>837</v>
+      </c>
+      <c r="G35" s="142" t="s">
+        <v>261</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>837</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="118" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="118" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" s="123">
+        <v>500</v>
+      </c>
+      <c r="G36" s="142" t="s">
+        <v>261</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="118" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="118" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="123">
+        <v>81</v>
+      </c>
+      <c r="G37" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H37">
+        <v>81</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="118" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="118" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="123">
+        <v>1000</v>
+      </c>
+      <c r="G38" s="142" t="s">
+        <v>261</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="118" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="118" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" s="123">
+        <v>598</v>
+      </c>
+      <c r="G39" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H39">
+        <v>598</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="118" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="118" t="s">
+        <v>127</v>
+      </c>
+      <c r="F40" s="123">
+        <v>2853.9</v>
+      </c>
+      <c r="G40" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H40">
+        <v>2853.9</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="118" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="118" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" s="123">
+        <v>378</v>
+      </c>
+      <c r="G41" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H41">
+        <v>378</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="118" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" s="118" t="s">
+        <v>231</v>
+      </c>
+      <c r="F42" s="123">
+        <v>811</v>
+      </c>
+      <c r="G42" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H42">
+        <v>811</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="118" t="s">
+        <v>255</v>
+      </c>
+      <c r="E43" s="118" t="s">
+        <v>256</v>
+      </c>
+      <c r="F43" s="123">
+        <v>914</v>
+      </c>
+      <c r="G43" s="142" t="s">
+        <v>266</v>
+      </c>
+      <c r="H43">
+        <v>914</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="17" thickBot="1">
+      <c r="B44" s="124" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="125" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="E44" s="125" t="s">
+        <v>260</v>
+      </c>
+      <c r="F44" s="126">
+        <v>1502.1</v>
+      </c>
+      <c r="G44" s="142" t="s">
+        <v>261</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>1502.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G31:G44">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="c">
+      <formula>NOT(ISERROR(SEARCH("c",G31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BF7A57-00C7-044C-A95A-5E3B0411BE36}">
   <dimension ref="B2:L66"/>
   <sheetViews>

</xml_diff>